<commit_message>
bought STM32 and wires
</commit_message>
<xml_diff>
--- a/Materiales.xlsx
+++ b/Materiales.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>COMPONENTES</t>
   </si>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +419,7 @@
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -430,23 +430,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3">
-        <v>603.71</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3">
-        <v>325.57</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -457,28 +463,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>